<commit_message>
Update Script & SCF 2025.2.2 Framework
</commit_message>
<xml_diff>
--- a/tools/excel/scf/scf-2025.2.2.xlsx
+++ b/tools/excel/scf/scf-2025.2.2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JulianDoloir\Desktop\Repos\intuitem\ciso-assistant-community\tools\excel\scf\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A14FF4CB-36D4-4FD8-8A2C-4FBCA9526A64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25B99E9A-8F10-494E-AE6A-454FC0C43E31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1485" yWindow="-15870" windowWidth="25440" windowHeight="15990" tabRatio="848" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1152" yWindow="1152" windowWidth="17976" windowHeight="11328" tabRatio="848" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="library_meta" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8149" uniqueCount="5450">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8182" uniqueCount="5483">
   <si>
     <t>type</t>
   </si>
@@ -17038,6 +17038,105 @@
   <si>
     <t>SCF: Secure Controls Framework
 https://securecontrolsframework.com/about-us/</t>
+  </si>
+  <si>
+    <t>GOV</t>
+  </si>
+  <si>
+    <t>AAT</t>
+  </si>
+  <si>
+    <t>AST</t>
+  </si>
+  <si>
+    <t>BCD</t>
+  </si>
+  <si>
+    <t>CAP</t>
+  </si>
+  <si>
+    <t>CHG</t>
+  </si>
+  <si>
+    <t>CLD</t>
+  </si>
+  <si>
+    <t>CPL</t>
+  </si>
+  <si>
+    <t>CFG</t>
+  </si>
+  <si>
+    <t>MON</t>
+  </si>
+  <si>
+    <t>CRY</t>
+  </si>
+  <si>
+    <t>DCH</t>
+  </si>
+  <si>
+    <t>EMB</t>
+  </si>
+  <si>
+    <t>END</t>
+  </si>
+  <si>
+    <t>HRS</t>
+  </si>
+  <si>
+    <t>IAC</t>
+  </si>
+  <si>
+    <t>IRO</t>
+  </si>
+  <si>
+    <t>IAO</t>
+  </si>
+  <si>
+    <t>MNT</t>
+  </si>
+  <si>
+    <t>MDM</t>
+  </si>
+  <si>
+    <t>NET</t>
+  </si>
+  <si>
+    <t>PES</t>
+  </si>
+  <si>
+    <t>PRI</t>
+  </si>
+  <si>
+    <t>PRM</t>
+  </si>
+  <si>
+    <t>RSK</t>
+  </si>
+  <si>
+    <t>SEA</t>
+  </si>
+  <si>
+    <t>OPS</t>
+  </si>
+  <si>
+    <t>SAT</t>
+  </si>
+  <si>
+    <t>TDA</t>
+  </si>
+  <si>
+    <t>TPM</t>
+  </si>
+  <si>
+    <t>THR</t>
+  </si>
+  <si>
+    <t>VPM</t>
+  </si>
+  <si>
+    <t>WEB</t>
   </si>
 </sst>
 </file>
@@ -17439,7 +17538,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -17637,9 +17736,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G1376"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A1377" sqref="A1377"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17680,6 +17779,9 @@
       <c r="B2">
         <v>1</v>
       </c>
+      <c r="C2" t="s">
+        <v>5450</v>
+      </c>
       <c r="D2" t="s">
         <v>41</v>
       </c>
@@ -18447,6 +18549,9 @@
       <c r="B36">
         <v>1</v>
       </c>
+      <c r="C36" t="s">
+        <v>5451</v>
+      </c>
       <c r="D36" t="s">
         <v>167</v>
       </c>
@@ -21059,6 +21164,9 @@
       <c r="B151">
         <v>1</v>
       </c>
+      <c r="C151" t="s">
+        <v>5452</v>
+      </c>
       <c r="D151" t="s">
         <v>421</v>
       </c>
@@ -22447,6 +22555,9 @@
       <c r="B212">
         <v>1</v>
       </c>
+      <c r="C212" t="s">
+        <v>5453</v>
+      </c>
       <c r="D212" t="s">
         <v>656</v>
       </c>
@@ -23789,6 +23900,9 @@
       <c r="B271">
         <v>1</v>
       </c>
+      <c r="C271" t="s">
+        <v>5454</v>
+      </c>
       <c r="D271" t="s">
         <v>879</v>
       </c>
@@ -23935,6 +24049,9 @@
       <c r="B278">
         <v>1</v>
       </c>
+      <c r="C278" t="s">
+        <v>5455</v>
+      </c>
       <c r="D278" t="s">
         <v>904</v>
       </c>
@@ -24380,6 +24497,9 @@
       <c r="B298">
         <v>1</v>
       </c>
+      <c r="C298" t="s">
+        <v>5456</v>
+      </c>
       <c r="D298" t="s">
         <v>973</v>
       </c>
@@ -24894,6 +25014,9 @@
       <c r="B321">
         <v>1</v>
       </c>
+      <c r="C321" t="s">
+        <v>5457</v>
+      </c>
       <c r="D321" t="s">
         <v>1062</v>
       </c>
@@ -25431,6 +25554,9 @@
       <c r="B345">
         <v>1</v>
       </c>
+      <c r="C345" t="s">
+        <v>5458</v>
+      </c>
       <c r="D345" t="s">
         <v>1129</v>
       </c>
@@ -26083,6 +26209,9 @@
       <c r="B374">
         <v>1</v>
       </c>
+      <c r="C374" t="s">
+        <v>5459</v>
+      </c>
       <c r="D374" t="s">
         <v>1240</v>
       </c>
@@ -27678,6 +27807,9 @@
       <c r="B444">
         <v>1</v>
       </c>
+      <c r="C444" t="s">
+        <v>5460</v>
+      </c>
       <c r="D444" t="s">
         <v>5286</v>
       </c>
@@ -28330,6 +28462,9 @@
       <c r="B473">
         <v>1</v>
       </c>
+      <c r="C473" t="s">
+        <v>5461</v>
+      </c>
       <c r="D473" t="s">
         <v>5287</v>
       </c>
@@ -30293,6 +30428,9 @@
       <c r="B559">
         <v>1</v>
       </c>
+      <c r="C559" t="s">
+        <v>5462</v>
+      </c>
       <c r="D559" t="s">
         <v>5290</v>
       </c>
@@ -30738,6 +30876,9 @@
       <c r="B579">
         <v>1</v>
       </c>
+      <c r="C579" t="s">
+        <v>5463</v>
+      </c>
       <c r="D579" t="s">
         <v>2036</v>
       </c>
@@ -31781,6 +31922,9 @@
       <c r="B625">
         <v>1</v>
       </c>
+      <c r="C625" t="s">
+        <v>5464</v>
+      </c>
       <c r="D625" t="s">
         <v>2215</v>
       </c>
@@ -32824,6 +32968,9 @@
       <c r="B671">
         <v>1</v>
       </c>
+      <c r="C671" t="s">
+        <v>5465</v>
+      </c>
       <c r="D671" t="s">
         <v>2380</v>
       </c>
@@ -35270,6 +35417,9 @@
       <c r="B778">
         <v>1</v>
       </c>
+      <c r="C778" t="s">
+        <v>5466</v>
+      </c>
       <c r="D778" t="s">
         <v>2797</v>
       </c>
@@ -36221,6 +36371,9 @@
       <c r="B820">
         <v>1</v>
       </c>
+      <c r="C820" t="s">
+        <v>5467</v>
+      </c>
       <c r="D820" t="s">
         <v>5343</v>
       </c>
@@ -36574,6 +36727,9 @@
       <c r="B836">
         <v>1</v>
       </c>
+      <c r="C836" t="s">
+        <v>5468</v>
+      </c>
       <c r="D836" t="s">
         <v>2995</v>
       </c>
@@ -37226,6 +37382,9 @@
       <c r="B865">
         <v>1</v>
       </c>
+      <c r="C865" t="s">
+        <v>5469</v>
+      </c>
       <c r="D865" t="s">
         <v>3108</v>
       </c>
@@ -37487,6 +37646,9 @@
       <c r="B877">
         <v>1</v>
       </c>
+      <c r="C877" t="s">
+        <v>5470</v>
+      </c>
       <c r="D877" t="s">
         <v>3153</v>
       </c>
@@ -39749,6 +39911,9 @@
       <c r="B976">
         <v>1</v>
       </c>
+      <c r="C976" t="s">
+        <v>5471</v>
+      </c>
       <c r="D976" t="s">
         <v>5349</v>
       </c>
@@ -40930,6 +41095,9 @@
       <c r="B1028">
         <v>1</v>
       </c>
+      <c r="C1028" t="s">
+        <v>5472</v>
+      </c>
       <c r="D1028" t="s">
         <v>3744</v>
       </c>
@@ -42778,6 +42946,9 @@
       <c r="B1109">
         <v>1</v>
       </c>
+      <c r="C1109" t="s">
+        <v>5473</v>
+      </c>
       <c r="D1109" t="s">
         <v>4046</v>
       </c>
@@ -43016,6 +43187,9 @@
       <c r="B1120">
         <v>1</v>
       </c>
+      <c r="C1120" t="s">
+        <v>5474</v>
+      </c>
       <c r="D1120" t="s">
         <v>4086</v>
       </c>
@@ -43599,6 +43773,9 @@
       <c r="B1146">
         <v>1</v>
       </c>
+      <c r="C1146" t="s">
+        <v>5475</v>
+      </c>
       <c r="D1146" t="s">
         <v>5378</v>
       </c>
@@ -44573,6 +44750,9 @@
       <c r="B1189">
         <v>1</v>
       </c>
+      <c r="C1189" t="s">
+        <v>5476</v>
+      </c>
       <c r="D1189" t="s">
         <v>4349</v>
       </c>
@@ -44765,6 +44945,9 @@
       <c r="B1198">
         <v>1</v>
       </c>
+      <c r="C1198" t="s">
+        <v>5477</v>
+      </c>
       <c r="D1198" t="s">
         <v>5379</v>
       </c>
@@ -45164,6 +45347,9 @@
       <c r="B1216">
         <v>1</v>
       </c>
+      <c r="C1216" t="s">
+        <v>5478</v>
+      </c>
       <c r="D1216" t="s">
         <v>4445</v>
       </c>
@@ -46707,6 +46893,9 @@
       <c r="B1284">
         <v>1</v>
       </c>
+      <c r="C1284" t="s">
+        <v>5479</v>
+      </c>
       <c r="D1284" t="s">
         <v>5435</v>
       </c>
@@ -47359,6 +47548,9 @@
       <c r="B1313">
         <v>1</v>
       </c>
+      <c r="C1313" t="s">
+        <v>5480</v>
+      </c>
       <c r="D1313" t="s">
         <v>4771</v>
       </c>
@@ -47666,6 +47858,9 @@
       <c r="B1327">
         <v>1</v>
       </c>
+      <c r="C1327" t="s">
+        <v>5481</v>
+      </c>
       <c r="D1327" t="s">
         <v>5440</v>
       </c>
@@ -48432,6 +48627,9 @@
     <row r="1361" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B1361">
         <v>1</v>
+      </c>
+      <c r="C1361" t="s">
+        <v>5482</v>
       </c>
       <c r="D1361" t="s">
         <v>4949</v>

</xml_diff>